<commit_message>
:sparkles: Implement create broadcast users
</commit_message>
<xml_diff>
--- a/src/assets/sample-file/broadcasts-import.xlsx
+++ b/src/assets/sample-file/broadcasts-import.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ade/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ade/Projects/ReactJs/save-me/src/assets/sample-file/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9BFF2A96-E85F-764D-AB58-20AEB13839E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E84FBD9-F8C1-ED48-866B-CE15EDA4F754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8100" yWindow="3300" windowWidth="27640" windowHeight="16940" xr2:uid="{E4954DFF-3440-E441-BB33-4EC330B8A653}"/>
+    <workbookView xWindow="5960" yWindow="3160" windowWidth="27640" windowHeight="16940" xr2:uid="{E4954DFF-3440-E441-BB33-4EC330B8A653}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,22 +40,22 @@
     <t>Name</t>
   </si>
   <si>
-    <t>whatsapp</t>
-  </si>
-  <si>
     <t>John Doe</t>
   </si>
   <si>
     <t>+6281234567890</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
     <t>test@gmail.com</t>
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Whatsapp</t>
+  </si>
+  <si>
+    <t>Email</t>
   </si>
 </sst>
 </file>
@@ -431,7 +431,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -444,16 +444,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -461,13 +461,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>